<commit_message>
Market refresh for AUD, HKD and JPY at 25-06-2015
</commit_message>
<xml_diff>
--- a/QuantLibXL/Data2/XLS/HKD/HKD_Market.xlsx
+++ b/QuantLibXL/Data2/XLS/HKD/HKD_Market.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="18585" yWindow="-15" windowWidth="18630" windowHeight="11010"/>
+    <workbookView xWindow="18585" yWindow="-15" windowWidth="18630" windowHeight="11010" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="General Settings" sheetId="40" r:id="rId1"/>
@@ -2066,68 +2066,68 @@
 <file path=xl/volatileDependencies.xml><?xml version="1.0" encoding="utf-8"?>
 <volTypes xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <volType type="realTimeData">
+    <main first="pldatasource.rhistoryrtdserver">
+      <tp t="s">
+        <v>Updated at 14:24:19</v>
+        <stp/>
+        <stp>{EBF2AD3F-1767-4A99-98FF-27FF13CB68B1}_x0000_</stp>
+        <tr r="E2" s="41"/>
+      </tp>
+    </main>
     <main first="pldatasource.rdatartdserver">
       <tp t="s">
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
         <stp/>
-        <stp>{722DEF7D-372D-4107-947A-25498D0D70AA}</stp>
+        <stp>{52DC35E4-373A-4739-B6F5-FE66A12C0601}</stp>
+        <tr r="O3" s="12"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:24:19</v>
+        <stp/>
+        <stp>{331CDCA1-DDF2-488E-A6BB-98441725FCD6}</stp>
+        <tr r="S4" s="43"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:24:20</v>
+        <stp/>
+        <stp>{274D53AE-7179-4AF7-85C7-CD725BDB8D22}</stp>
+        <tr r="T5" s="36"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:24:20</v>
+        <stp/>
+        <stp>{5B28EA16-A474-41E9-ABA8-DE07F99A4B6A}</stp>
+        <tr r="I3" s="9"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:24:19</v>
+        <stp/>
+        <stp>{0E41D8CC-32F6-4B25-A5C2-E3182527E604}</stp>
+        <tr r="L4" s="16"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:24:19</v>
+        <stp/>
+        <stp>{5E3F4C33-D422-44C1-8090-DF275CF1870B}</stp>
+        <tr r="L4" s="19"/>
+      </tp>
+      <tp t="s">
+        <v>Updated at 14:24:19</v>
+        <stp/>
+        <stp>{3B4AAED4-FAB1-4771-BC97-6693887D0DF6}</stp>
         <tr r="S4" s="5"/>
       </tp>
       <tp t="s">
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
         <stp/>
-        <stp>{C1300B64-FF7D-4B80-BFAD-15BDDCE3657E}</stp>
-        <tr r="L4" s="16"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 11:12:44</v>
-        <stp/>
-        <stp>{762679A3-71F7-417C-AFCD-A7BCFF0797AB}</stp>
-        <tr r="S4" s="43"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 11:12:44</v>
-        <stp/>
-        <stp>{245E250E-6938-48F4-8AC0-E5B80683F6D7}</stp>
+        <stp>{BD438690-9FA6-4DC3-876F-9F141EA07261}</stp>
         <tr r="M4" s="10"/>
       </tp>
       <tp t="s">
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
         <stp/>
-        <stp>{4204A290-C821-41B7-9A22-2774DB238F6F}</stp>
+        <stp>{9BF74A3D-CCE0-4DC6-BE34-5A017E88E9B2}</stp>
         <tr r="L4" s="17"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 11:12:44</v>
-        <stp/>
-        <stp>{21D18F73-7638-4DB6-9799-D37E2DF93040}</stp>
-        <tr r="L4" s="19"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 11:12:44</v>
-        <stp/>
-        <stp>{83F41C27-75D9-46DC-9EE1-97F346513EAC}</stp>
-        <tr r="I3" s="9"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 11:12:45</v>
-        <stp/>
-        <stp>{6437F67D-2EDA-43DA-B15F-68CF29B5EBF5}</stp>
-        <tr r="O3" s="12"/>
-      </tp>
-      <tp t="s">
-        <v>Paused at 11:12:44</v>
-        <stp/>
-        <stp>{A5B83699-E1DE-4463-8FAF-75FDE9F03EF5}</stp>
-        <tr r="T5" s="36"/>
-      </tp>
-    </main>
-    <main first="pldatasource.rhistoryrtdserver">
-      <tp t="s">
-        <v>Paused at 11:12:45</v>
-        <stp/>
-        <stp>{BFC783C0-6BF0-4B2B-B15A-AC0E4B87651F}_x0000_</stp>
-        <tr r="E2" s="41"/>
       </tp>
     </main>
   </volType>
@@ -2424,7 +2424,7 @@
   <sheetPr codeName="HKD_InterestRateQuotesFeed"/>
   <dimension ref="B1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -2440,7 +2440,7 @@
     <row r="1" spans="2:5" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="235" t="str">
         <f>_xll.qlxlVersion(TRUE,Trigger)</f>
-        <v>QuantLibXL 1.6.0 - MS VC++ (version unknown) - Multithreaded Dynamic Runtime library - Release Configuration - Jun 25 2015 08:49:52</v>
+        <v>QuantLibXL 1.6.0 - MS VC++ 9.0 - Multithreaded Dynamic Runtime library - Release Configuration - Jun 18 2015 16:49:40</v>
       </c>
     </row>
     <row r="2" spans="2:5" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2463,7 +2463,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="237">
-        <v>42180.467187499999</v>
+        <v>42180.600219907406</v>
       </c>
       <c r="E4" s="238"/>
     </row>
@@ -2479,7 +2479,7 @@
         <v>169</v>
       </c>
       <c r="D6" s="239">
-        <v>42135.760763888888</v>
+        <v>42180.600462962961</v>
       </c>
       <c r="E6" s="238"/>
     </row>
@@ -2625,7 +2625,7 @@
       </c>
       <c r="D22" s="247">
         <f>_xll.ohTrigger(ISERROR(OIS!V3),ISERROR(Deposits!O2),ISERROR(FRA!W3),ISERROR(Futures3M!Z2),ISERROR(Swaps1M!V3),ISERROR(Swap3M!V3),ISERROR(BasisSwap1M3M!AB3),ISERROR(#REF!),ISERROR('Hibor Time Series'!J5:L13))</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E22" s="38"/>
     </row>
@@ -2894,7 +2894,7 @@
       <c r="AA3" s="146"/>
       <c r="AB3" s="107">
         <f>_xll.ohTrigger(AB5:AB43)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AC3" s="84"/>
       <c r="AD3" s="116"/>
@@ -2932,7 +2932,7 @@
       <c r="R4" s="143"/>
       <c r="S4" s="106" t="str">
         <f>_xll.RData(S5:S43,T4:U4,,ReutersRtMode,,T5)</f>
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
       </c>
       <c r="T4" s="142" t="s">
         <v>157</v>
@@ -3029,9 +3029,9 @@
         <f t="array" ref="AA5:AA43">QuoteLive</f>
         <v>15</v>
       </c>
-      <c r="AB5" s="94" t="e">
+      <c r="AB5" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z5,ROUND($AA5/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC5" s="84"/>
       <c r="AD5" s="116"/>
@@ -3109,9 +3109,9 @@
       <c r="AA6" s="194">
         <v>15</v>
       </c>
-      <c r="AB6" s="94" t="e">
+      <c r="AB6" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z6,ROUND($AA6/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="84"/>
       <c r="AD6" s="116"/>
@@ -3189,9 +3189,9 @@
       <c r="AA7" s="194">
         <v>15</v>
       </c>
-      <c r="AB7" s="94" t="e">
+      <c r="AB7" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z7,ROUND($AA7/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="84"/>
       <c r="AD7" s="116"/>
@@ -3349,9 +3349,9 @@
       <c r="AA9" s="194">
         <v>15</v>
       </c>
-      <c r="AB9" s="94" t="e">
+      <c r="AB9" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z9,ROUND($AA9/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="84"/>
       <c r="AD9" s="116"/>
@@ -3500,18 +3500,18 @@
         <v>HKD3HI1HI2Y=PREA</v>
       </c>
       <c r="T11" s="197">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="U11" s="197">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="V11" s="196">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="W11" s="88"/>
       <c r="X11" s="195">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="Y11" s="88"/>
       <c r="Z11" s="96" t="str">
@@ -3519,11 +3519,11 @@
         <v>HKD3HI1HI2Y_Quote</v>
       </c>
       <c r="AA11" s="194">
-        <v>15</v>
-      </c>
-      <c r="AB11" s="94" t="e">
+        <v>14</v>
+      </c>
+      <c r="AB11" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z11,ROUND($AA11/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>-1.0000000000000005E-4</v>
       </c>
       <c r="AC11" s="84"/>
       <c r="AD11" s="116"/>
@@ -3583,18 +3583,18 @@
         <v>HKD3HI1HI3Y=PREA</v>
       </c>
       <c r="T12" s="197">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U12" s="197">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V12" s="196">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="W12" s="88"/>
       <c r="X12" s="195">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Y12" s="88"/>
       <c r="Z12" s="96" t="str">
@@ -3602,11 +3602,11 @@
         <v>HKD3HI1HI3Y_Quote</v>
       </c>
       <c r="AA12" s="194">
-        <v>13</v>
-      </c>
-      <c r="AB12" s="94" t="e">
+        <v>14</v>
+      </c>
+      <c r="AB12" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z12,ROUND($AA12/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>1.0000000000000005E-4</v>
       </c>
       <c r="AC12" s="84"/>
       <c r="AD12" s="116"/>
@@ -3666,18 +3666,18 @@
         <v>HKD3HI1HI4Y=PREA</v>
       </c>
       <c r="T13" s="197">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="U13" s="197">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="V13" s="196">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="W13" s="88"/>
       <c r="X13" s="195">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Y13" s="88"/>
       <c r="Z13" s="96" t="str">
@@ -3685,11 +3685,11 @@
         <v>HKD3HI1HI4Y_Quote</v>
       </c>
       <c r="AA13" s="194">
-        <v>12</v>
-      </c>
-      <c r="AB13" s="94" t="e">
+        <v>14</v>
+      </c>
+      <c r="AB13" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z13,ROUND($AA13/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>2.0000000000000009E-4</v>
       </c>
       <c r="AC13" s="84"/>
       <c r="AD13" s="116"/>
@@ -3749,18 +3749,18 @@
         <v>HKD3HI1HI5Y=PREA</v>
       </c>
       <c r="T14" s="197">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="U14" s="197">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="V14" s="196">
         <f t="shared" si="4"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="W14" s="88"/>
       <c r="X14" s="195">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Y14" s="88"/>
       <c r="Z14" s="96" t="str">
@@ -3768,11 +3768,11 @@
         <v>HKD3HI1HI5Y_Quote</v>
       </c>
       <c r="AA14" s="194">
-        <v>12</v>
-      </c>
-      <c r="AB14" s="94" t="e">
+        <v>14</v>
+      </c>
+      <c r="AB14" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z14,ROUND($AA14/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>2.0000000000000009E-4</v>
       </c>
       <c r="AC14" s="84"/>
       <c r="AD14" s="116"/>
@@ -3918,9 +3918,9 @@
       <c r="AA16" s="194">
         <v>8</v>
       </c>
-      <c r="AB16" s="94" t="e">
+      <c r="AB16" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z16,ROUND($AA16/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC16" s="84"/>
       <c r="AD16" s="116"/>
@@ -4140,9 +4140,9 @@
       <c r="AA19" s="194">
         <v>7</v>
       </c>
-      <c r="AB19" s="94" t="e">
+      <c r="AB19" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z19,ROUND($AA19/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="84"/>
       <c r="AD19" s="116"/>
@@ -4288,9 +4288,9 @@
       <c r="AA21" s="194">
         <v>4</v>
       </c>
-      <c r="AB21" s="94" t="e">
+      <c r="AB21" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z21,ROUND($AA21/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC21" s="84"/>
       <c r="AD21" s="116"/>
@@ -4510,9 +4510,9 @@
       <c r="AA24" s="194">
         <v>4</v>
       </c>
-      <c r="AB24" s="94" t="e">
+      <c r="AB24" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z24,ROUND($AA24/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC24" s="84"/>
       <c r="AD24" s="116"/>
@@ -6106,7 +6106,7 @@
       <c r="AA3" s="146"/>
       <c r="AB3" s="107">
         <f>_xll.ohTrigger(AB5:AB43)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AC3" s="84"/>
       <c r="AD3" s="116"/>
@@ -6144,7 +6144,7 @@
       <c r="R4" s="143"/>
       <c r="S4" s="106" t="str">
         <f>_xll.RData(S5:S43,T4:U4,,ReutersRtMode,,T5)</f>
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
       </c>
       <c r="T4" s="142" t="s">
         <v>157</v>
@@ -6241,9 +6241,9 @@
         <f t="array" ref="AA5:AA43">QuoteLive</f>
         <v>-16</v>
       </c>
-      <c r="AB5" s="94" t="e">
+      <c r="AB5" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z5,ROUND($AA5/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC5" s="84"/>
       <c r="AD5" s="116"/>
@@ -6321,9 +6321,9 @@
       <c r="AA6" s="194">
         <v>-15</v>
       </c>
-      <c r="AB6" s="94" t="e">
+      <c r="AB6" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z6,ROUND($AA6/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="84"/>
       <c r="AD6" s="116"/>
@@ -6401,9 +6401,9 @@
       <c r="AA7" s="194">
         <v>-15</v>
       </c>
-      <c r="AB7" s="94" t="e">
+      <c r="AB7" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z7,ROUND($AA7/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="84"/>
       <c r="AD7" s="116"/>
@@ -6561,9 +6561,9 @@
       <c r="AA9" s="194">
         <v>-14</v>
       </c>
-      <c r="AB9" s="94" t="e">
+      <c r="AB9" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z9,ROUND($AA9/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC9" s="84"/>
       <c r="AD9" s="116"/>
@@ -6733,9 +6733,9 @@
       <c r="AA11" s="194">
         <v>-14</v>
       </c>
-      <c r="AB11" s="94" t="e">
+      <c r="AB11" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z11,ROUND($AA11/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC11" s="84"/>
       <c r="AD11" s="116"/>
@@ -6816,9 +6816,9 @@
       <c r="AA12" s="194">
         <v>-13</v>
       </c>
-      <c r="AB12" s="94" t="e">
+      <c r="AB12" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z12,ROUND($AA12/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="84"/>
       <c r="AD12" s="116"/>
@@ -6899,9 +6899,9 @@
       <c r="AA13" s="194">
         <v>-12</v>
       </c>
-      <c r="AB13" s="94" t="e">
+      <c r="AB13" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z13,ROUND($AA13/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="84"/>
       <c r="AD13" s="116"/>
@@ -6982,9 +6982,9 @@
       <c r="AA14" s="194">
         <v>-11</v>
       </c>
-      <c r="AB14" s="94" t="e">
+      <c r="AB14" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z14,ROUND($AA14/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="84"/>
       <c r="AD14" s="116"/>
@@ -7130,9 +7130,9 @@
       <c r="AA16" s="194">
         <v>-10</v>
       </c>
-      <c r="AB16" s="94" t="e">
+      <c r="AB16" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z16,ROUND($AA16/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC16" s="84"/>
       <c r="AD16" s="116"/>
@@ -7352,9 +7352,9 @@
       <c r="AA19" s="194">
         <v>-10</v>
       </c>
-      <c r="AB19" s="94" t="e">
+      <c r="AB19" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z19,ROUND($AA19/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="84"/>
       <c r="AD19" s="116"/>
@@ -7500,9 +7500,9 @@
       <c r="AA21" s="194">
         <v>-11</v>
       </c>
-      <c r="AB21" s="94" t="e">
+      <c r="AB21" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z21,ROUND($AA21/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC21" s="84"/>
       <c r="AD21" s="116"/>
@@ -7722,9 +7722,9 @@
       <c r="AA24" s="194">
         <v>-11</v>
       </c>
-      <c r="AB24" s="94" t="e">
+      <c r="AB24" s="94">
         <f>_xll.qlSimpleQuoteSetValue($Z24,ROUND($AA24/10000,6),Trigger)</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="AC24" s="84"/>
       <c r="AD24" s="116"/>
@@ -9377,7 +9377,7 @@
       </c>
       <c r="T5" s="211" t="str">
         <f>_xll.RData(T6:T14,U5:V5,"RTFEED:IDN",,,U6)</f>
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:20</v>
       </c>
       <c r="U5" s="211" t="s">
         <v>173</v>
@@ -9457,10 +9457,10 @@
         <v>HIHKDOND=</v>
       </c>
       <c r="U6" s="209">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="V6" s="225">
-        <v>4.7990000000000005E-2</v>
+        <v>5.6530000000000004E-2</v>
       </c>
       <c r="W6" s="208" t="b">
         <f t="shared" ref="W6:W14" si="2">IF(AND(ISNUMBER($V6),$V6&lt;&gt;0%),TRUE,FALSE)</f>
@@ -9472,7 +9472,7 @@
       </c>
       <c r="Y6" s="228">
         <f>_xll.qlQuoteValue(M6,X6)</f>
-        <v>4.7990000000000006E-4</v>
+        <v>5.6530000000000003E-4</v>
       </c>
       <c r="Z6" s="259"/>
     </row>
@@ -9509,11 +9509,11 @@
       </c>
       <c r="L7" s="266" t="str">
         <f>_xll.qlIborIndex(J7,FamilyName,D7,E7,Currency,F7,G7,H7,I7,K7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHiborSW#0006</v>
+        <v>HkdHiborSW#0001</v>
       </c>
       <c r="M7" s="267" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C7&amp;"LastFixing_Quote",L7,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHiborSWLastFixing_Quote#0006</v>
+        <v>HkdHiborSWLastFixing_Quote#0001</v>
       </c>
       <c r="N7" s="258" t="str">
         <f>_xll.ohRangeRetrieveError(L7)</f>
@@ -9528,17 +9528,17 @@
       </c>
       <c r="S7" s="204" t="str">
         <f t="shared" ref="S7:S14" si="3">IFERROR(L7,J7)</f>
-        <v>HkdHiborSW#0006</v>
+        <v>HkdHiborSW#0001</v>
       </c>
       <c r="T7" s="204" t="str">
         <f t="shared" si="1"/>
         <v>HIHKD1WD=</v>
       </c>
       <c r="U7" s="206">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="V7" s="226">
-        <v>9.9140000000000006E-2</v>
+        <v>0.11600000000000001</v>
       </c>
       <c r="W7" s="205" t="b">
         <f t="shared" si="2"/>
@@ -9550,7 +9550,7 @@
       </c>
       <c r="Y7" s="229">
         <f>_xll.qlQuoteValue(M7,X7)</f>
-        <v>9.9140000000000014E-4</v>
+        <v>1.16E-3</v>
       </c>
       <c r="Z7" s="259"/>
     </row>
@@ -9588,11 +9588,11 @@
       </c>
       <c r="L8" s="266" t="str">
         <f>_xll.qlIborIndex(J8,FamilyName,D8,E8,Currency,F8,G8,H8,I8,K8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor2W#0003</v>
+        <v>HkdHibor2W#0001</v>
       </c>
       <c r="M8" s="267" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C8&amp;"LastFixing_Quote",L8,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor2WLastFixing_Quote#0003</v>
+        <v>HkdHibor2WLastFixing_Quote#0001</v>
       </c>
       <c r="N8" s="258" t="str">
         <f>_xll.ohRangeRetrieveError(L8)</f>
@@ -9608,17 +9608,17 @@
       </c>
       <c r="S8" s="204" t="str">
         <f t="shared" si="3"/>
-        <v>HkdHibor2W#0003</v>
+        <v>HkdHibor2W#0001</v>
       </c>
       <c r="T8" s="204" t="str">
         <f t="shared" si="1"/>
         <v>HIHKD2WD=</v>
       </c>
       <c r="U8" s="206">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="V8" s="226">
-        <v>0.13820000000000002</v>
+        <v>0.16257000000000002</v>
       </c>
       <c r="W8" s="205" t="b">
         <f t="shared" si="2"/>
@@ -9630,7 +9630,7 @@
       </c>
       <c r="Y8" s="229">
         <f>_xll.qlQuoteValue(M8,X8)</f>
-        <v>1.3820000000000002E-3</v>
+        <v>1.6257000000000001E-3</v>
       </c>
       <c r="Z8" s="259"/>
     </row>
@@ -9668,11 +9668,11 @@
       </c>
       <c r="L9" s="266" t="str">
         <f>_xll.qlIborIndex(J9,FamilyName,D9,E9,Currency,F9,G9,H9,I9,K9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor1M#0003</v>
+        <v>HkdHibor1M#0001</v>
       </c>
       <c r="M9" s="267" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C9&amp;"LastFixing_Quote",L9,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor1MLastFixing_Quote#0003</v>
+        <v>HkdHibor1MLastFixing_Quote#0001</v>
       </c>
       <c r="N9" s="258" t="str">
         <f>_xll.ohRangeRetrieveError(L9)</f>
@@ -9688,17 +9688,17 @@
       </c>
       <c r="S9" s="204" t="str">
         <f t="shared" si="3"/>
-        <v>HkdHibor1M#0003</v>
+        <v>HkdHibor1M#0001</v>
       </c>
       <c r="T9" s="204" t="str">
         <f t="shared" si="1"/>
         <v>HIHKD1MD=</v>
       </c>
       <c r="U9" s="206">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="V9" s="226">
-        <v>0.24043000000000003</v>
+        <v>0.24094000000000002</v>
       </c>
       <c r="W9" s="205" t="b">
         <f t="shared" si="2"/>
@@ -9710,7 +9710,7 @@
       </c>
       <c r="Y9" s="229">
         <f>_xll.qlQuoteValue(M9,X9)</f>
-        <v>2.4043000000000003E-3</v>
+        <v>2.4094000000000003E-3</v>
       </c>
       <c r="Z9" s="259"/>
     </row>
@@ -9748,11 +9748,11 @@
       </c>
       <c r="L10" s="266" t="str">
         <f>_xll.qlIborIndex(J10,FamilyName,D10,E10,Currency,F10,G10,H10,I10,K10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor2M#0003</v>
+        <v>HkdHibor2M#0001</v>
       </c>
       <c r="M10" s="267" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C10&amp;"LastFixing_Quote",L10,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor2MLastFixing_Quote#0003</v>
+        <v>HkdHibor2MLastFixing_Quote#0001</v>
       </c>
       <c r="N10" s="258" t="str">
         <f>_xll.ohRangeRetrieveError(L10)</f>
@@ -9768,17 +9768,17 @@
       </c>
       <c r="S10" s="204" t="str">
         <f t="shared" si="3"/>
-        <v>HkdHibor2M#0003</v>
+        <v>HkdHibor2M#0001</v>
       </c>
       <c r="T10" s="204" t="str">
         <f t="shared" si="1"/>
         <v>HIHKD2MD=</v>
       </c>
       <c r="U10" s="206">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="V10" s="226">
-        <v>0.30371000000000004</v>
+        <v>0.30586000000000002</v>
       </c>
       <c r="W10" s="205" t="b">
         <f t="shared" si="2"/>
@@ -9790,7 +9790,7 @@
       </c>
       <c r="Y10" s="229">
         <f>_xll.qlQuoteValue(M10,X10)</f>
-        <v>3.0371000000000005E-3</v>
+        <v>3.0586000000000003E-3</v>
       </c>
       <c r="Z10" s="259"/>
     </row>
@@ -9828,11 +9828,11 @@
       </c>
       <c r="L11" s="266" t="str">
         <f>_xll.qlIborIndex(J11,FamilyName,D11,E11,Currency,F11,G11,H11,I11,K11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor3M#0003</v>
+        <v>HkdHibor3M#0001</v>
       </c>
       <c r="M11" s="267" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C11&amp;"LastFixing_Quote",L11,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor3MLastFixing_Quote#0003</v>
+        <v>HkdHibor3MLastFixing_Quote#0001</v>
       </c>
       <c r="N11" s="258" t="str">
         <f>_xll.ohRangeRetrieveError(L11)</f>
@@ -9848,17 +9848,17 @@
       </c>
       <c r="S11" s="204" t="str">
         <f t="shared" si="3"/>
-        <v>HkdHibor3M#0003</v>
+        <v>HkdHibor3M#0001</v>
       </c>
       <c r="T11" s="204" t="str">
         <f t="shared" si="1"/>
         <v>HIHKD3MD=</v>
       </c>
       <c r="U11" s="206">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="V11" s="226">
-        <v>0.38600000000000001</v>
+        <v>0.38814000000000004</v>
       </c>
       <c r="W11" s="205" t="b">
         <f t="shared" si="2"/>
@@ -9870,7 +9870,7 @@
       </c>
       <c r="Y11" s="229">
         <f>_xll.qlQuoteValue(M11,X11)</f>
-        <v>3.8600000000000001E-3</v>
+        <v>3.8814000000000006E-3</v>
       </c>
       <c r="Z11" s="259"/>
     </row>
@@ -9908,11 +9908,11 @@
       </c>
       <c r="L12" s="266" t="str">
         <f>_xll.qlIborIndex(J12,FamilyName,D12,E12,Currency,F12,G12,H12,I12,K12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor6M#0003</v>
+        <v>HkdHibor6M#0001</v>
       </c>
       <c r="M12" s="267" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C12&amp;"LastFixing_Quote",L12,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor6MLastFixing_Quote#0003</v>
+        <v>HkdHibor6MLastFixing_Quote#0001</v>
       </c>
       <c r="N12" s="258" t="str">
         <f>_xll.ohRangeRetrieveError(L12)</f>
@@ -9928,17 +9928,17 @@
       </c>
       <c r="S12" s="204" t="str">
         <f t="shared" si="3"/>
-        <v>HkdHibor6M#0003</v>
+        <v>HkdHibor6M#0001</v>
       </c>
       <c r="T12" s="204" t="str">
         <f t="shared" si="1"/>
         <v>HIHKD6MD=</v>
       </c>
       <c r="U12" s="206">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="V12" s="226">
-        <v>0.54136000000000006</v>
+        <v>0.54286000000000001</v>
       </c>
       <c r="W12" s="205" t="b">
         <f t="shared" si="2"/>
@@ -9950,7 +9950,7 @@
       </c>
       <c r="Y12" s="229">
         <f>_xll.qlQuoteValue(M12,X12)</f>
-        <v>5.4136000000000011E-3</v>
+        <v>5.4286000000000004E-3</v>
       </c>
       <c r="Z12" s="259"/>
     </row>
@@ -9988,11 +9988,11 @@
       </c>
       <c r="L13" s="266" t="str">
         <f>_xll.qlIborIndex(J13,FamilyName,D13,E13,Currency,F13,G13,H13,I13,K13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor9M#0003</v>
+        <v>HkdHibor9M#0001</v>
       </c>
       <c r="M13" s="267" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C13&amp;"LastFixing_Quote",L13,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor9MLastFixing_Quote#0003</v>
+        <v>HkdHibor9MLastFixing_Quote#0001</v>
       </c>
       <c r="N13" s="258" t="str">
         <f>_xll.ohRangeRetrieveError(L13)</f>
@@ -10008,7 +10008,7 @@
       </c>
       <c r="S13" s="204" t="str">
         <f t="shared" si="3"/>
-        <v>HkdHibor9M#0003</v>
+        <v>HkdHibor9M#0001</v>
       </c>
       <c r="T13" s="204" t="str">
         <f t="shared" si="1"/>
@@ -10068,11 +10068,11 @@
       </c>
       <c r="L14" s="266" t="str">
         <f>_xll.qlIborIndex(J14,FamilyName,D14,E14,Currency,F14,G14,H14,I14,K14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor1Y#0003</v>
+        <v>HkdHibor1Y#0001</v>
       </c>
       <c r="M14" s="267" t="str">
         <f>_xll.qlLastFixingQuote(PROPER(Currency)&amp;FamilyName&amp;$C14&amp;"LastFixing_Quote",L14,Permanent,Trigger,ObjectOverwrite)</f>
-        <v>HkdHibor1YLastFixing_Quote#0003</v>
+        <v>HkdHibor1YLastFixing_Quote#0001</v>
       </c>
       <c r="N14" s="258" t="str">
         <f>_xll.ohRangeRetrieveError(L14)</f>
@@ -10088,17 +10088,17 @@
       </c>
       <c r="S14" s="201" t="str">
         <f t="shared" si="3"/>
-        <v>HkdHibor1Y#0003</v>
+        <v>HkdHibor1Y#0001</v>
       </c>
       <c r="T14" s="201" t="str">
         <f t="shared" si="1"/>
         <v>HIHKD1YD=</v>
       </c>
       <c r="U14" s="203">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="V14" s="227">
-        <v>0.84153000000000011</v>
+        <v>0.8432900000000001</v>
       </c>
       <c r="W14" s="202" t="b">
         <f t="shared" si="2"/>
@@ -10110,7 +10110,7 @@
       </c>
       <c r="Y14" s="230">
         <f>_xll.qlQuoteValue(M14,X14)</f>
-        <v>8.4153000000000006E-3</v>
+        <v>8.4329000000000001E-3</v>
       </c>
       <c r="Z14" s="259"/>
     </row>
@@ -10238,16 +10238,16 @@
     <row r="2" spans="1:190" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B2" s="298">
         <f>MIN(E5:E271)</f>
-        <v>41799</v>
+        <v>42170</v>
       </c>
       <c r="C2" s="298">
         <f>MAX(E5:E271)</f>
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="D2" s="299"/>
       <c r="E2" s="300" t="str">
         <f>_xll.RHistory(F2:H2,B8:C8,C3,,"CH:In;Fd TSREPEAT:N SORT:"&amp;C7,E3)</f>
-        <v>Paused at 11:12:45</v>
+        <v>Updated at 14:24:19</v>
       </c>
       <c r="F2" s="301" t="s">
         <v>194</v>
@@ -10495,16 +10495,16 @@
       </c>
       <c r="D5" s="307"/>
       <c r="E5" s="312">
-        <v>42135</v>
+        <v>42180</v>
       </c>
       <c r="F5" s="313">
-        <v>0.24043</v>
+        <v>0.24093999999999999</v>
       </c>
       <c r="G5" s="313">
-        <v>0.38600000000000001</v>
+        <v>0.38813999999999999</v>
       </c>
       <c r="H5" s="314">
-        <v>0.54135999999999995</v>
+        <v>0.54286000000000001</v>
       </c>
       <c r="J5" s="296" t="b">
         <f>IF(AND(ISNUMBER($E5),ISNUMBER(F5),Trigger),_xll.qlIndexAddFixings(J$3,$E5,F5/100,TRUE),NA())</f>
@@ -10522,16 +10522,16 @@
     <row r="6" spans="1:190" x14ac:dyDescent="0.2">
       <c r="D6" s="315"/>
       <c r="E6" s="312">
-        <v>42132</v>
+        <v>42179</v>
       </c>
       <c r="F6" s="313">
-        <v>0.23971000000000001</v>
+        <v>0.24013999999999999</v>
       </c>
       <c r="G6" s="313">
-        <v>0.38671</v>
+        <v>0.38743</v>
       </c>
       <c r="H6" s="314">
-        <v>0.54276999999999997</v>
+        <v>0.54213999999999996</v>
       </c>
       <c r="J6" s="296" t="b">
         <f>IF(AND(ISNUMBER($E6),ISNUMBER(F6),Trigger),_xll.qlIndexAddFixings(J$3,$E6,F6/100,TRUE),NA())</f>
@@ -10554,16 +10554,16 @@
         <v>190</v>
       </c>
       <c r="E7" s="312">
-        <v>42131</v>
+        <v>42178</v>
       </c>
       <c r="F7" s="313">
-        <v>0.23757</v>
+        <v>0.23971000000000001</v>
       </c>
       <c r="G7" s="313">
-        <v>0.38743</v>
+        <v>0.39015</v>
       </c>
       <c r="H7" s="314">
-        <v>0.54142999999999997</v>
+        <v>0.54213999999999996</v>
       </c>
       <c r="J7" s="296" t="b">
         <f>IF(AND(ISNUMBER($E7),ISNUMBER(F7),Trigger),_xll.qlIndexAddFixings(J$3,$E7,F7/100,TRUE),NA())</f>
@@ -10586,16 +10586,16 @@
         <v>192</v>
       </c>
       <c r="E8" s="312">
-        <v>42130</v>
+        <v>42177</v>
       </c>
       <c r="F8" s="313">
-        <v>0.23543</v>
+        <v>0.23783000000000001</v>
       </c>
       <c r="G8" s="313">
         <v>0.38600000000000001</v>
       </c>
       <c r="H8" s="314">
-        <v>0.54213999999999996</v>
+        <v>0.54</v>
       </c>
       <c r="J8" s="296" t="b">
         <f>IF(AND(ISNUMBER($E8),ISNUMBER(F8),Trigger),_xll.qlIndexAddFixings(J$3,$E8,F8/100,TRUE),NA())</f>
@@ -10614,16 +10614,16 @@
       <c r="B9" s="317"/>
       <c r="C9" s="317"/>
       <c r="E9" s="312">
-        <v>42129</v>
+        <v>42174</v>
       </c>
       <c r="F9" s="313">
-        <v>0.23685999999999999</v>
+        <v>0.23779</v>
       </c>
       <c r="G9" s="313">
-        <v>0.38600000000000001</v>
+        <v>0.38671</v>
       </c>
       <c r="H9" s="314">
-        <v>0.54286000000000001</v>
+        <v>0.53929000000000005</v>
       </c>
       <c r="J9" s="296" t="b">
         <f>IF(AND(ISNUMBER($E9),ISNUMBER(F9),Trigger),_xll.qlIndexAddFixings(J$3,$E9,F9/100,TRUE),NA())</f>
@@ -10640,16 +10640,16 @@
     </row>
     <row r="10" spans="1:190" x14ac:dyDescent="0.2">
       <c r="E10" s="312">
-        <v>42128</v>
+        <v>42173</v>
       </c>
       <c r="F10" s="313">
-        <v>0.23929</v>
+        <v>0.23823</v>
       </c>
       <c r="G10" s="313">
-        <v>0.38357000000000002</v>
+        <v>0.38885999999999998</v>
       </c>
       <c r="H10" s="314">
-        <v>0.54213999999999996</v>
+        <v>0.54071000000000002</v>
       </c>
       <c r="J10" s="296" t="b">
         <f>IF(AND(ISNUMBER($E10),ISNUMBER(F10),Trigger),_xll.qlIndexAddFixings(J$3,$E10,F10/100,TRUE),NA())</f>
@@ -10666,16 +10666,16 @@
     </row>
     <row r="11" spans="1:190" x14ac:dyDescent="0.2">
       <c r="E11" s="312">
-        <v>41810</v>
+        <v>42172</v>
       </c>
       <c r="F11" s="313">
-        <v>0.21429000000000001</v>
+        <v>0.23757</v>
       </c>
       <c r="G11" s="313">
-        <v>0.37642999999999999</v>
+        <v>0.38885999999999998</v>
       </c>
       <c r="H11" s="314">
-        <v>0.55071000000000003</v>
+        <v>0.54071000000000002</v>
       </c>
       <c r="J11" s="296" t="b">
         <f>IF(AND(ISNUMBER($E11),ISNUMBER(F11),Trigger),_xll.qlIndexAddFixings(J$3,$E11,F11/100,TRUE),NA())</f>
@@ -10692,16 +10692,16 @@
     </row>
     <row r="12" spans="1:190" x14ac:dyDescent="0.2">
       <c r="E12" s="312">
-        <v>41800</v>
+        <v>42171</v>
       </c>
       <c r="F12" s="313">
-        <v>0.20751</v>
+        <v>0.24113999999999999</v>
       </c>
       <c r="G12" s="313">
-        <v>0.37184</v>
+        <v>0.39100000000000001</v>
       </c>
       <c r="H12" s="314">
-        <v>0.54786000000000001</v>
+        <v>0.54142999999999997</v>
       </c>
       <c r="J12" s="296" t="b">
         <f>IF(AND(ISNUMBER($E12),ISNUMBER(F12),Trigger),_xll.qlIndexAddFixings(J$3,$E12,F12/100,TRUE),NA())</f>
@@ -10718,16 +10718,16 @@
     </row>
     <row r="13" spans="1:190" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E13" s="312">
-        <v>41799</v>
+        <v>42170</v>
       </c>
       <c r="F13" s="313">
-        <v>0.20912</v>
+        <v>0.23921000000000001</v>
       </c>
       <c r="G13" s="313">
-        <v>0.37125999999999998</v>
+        <v>0.39029000000000003</v>
       </c>
       <c r="H13" s="314">
-        <v>0.54928999999999994</v>
+        <v>0.54213999999999996</v>
       </c>
       <c r="J13" s="296" t="b">
         <f>IF(AND(ISNUMBER($E13),ISNUMBER(F13),Trigger),_xll.qlIndexAddFixings(J$3,$E13,F13/100,TRUE),NA())</f>
@@ -12923,7 +12923,7 @@
       <c r="U3" s="146"/>
       <c r="V3" s="107">
         <f>_xll.ohTrigger(V5:V23)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="W3" s="84"/>
       <c r="X3" s="281"/>
@@ -12952,7 +12952,7 @@
       <c r="K4" s="145"/>
       <c r="L4" s="106" t="str">
         <f>_xll.RData(L5:L23,M4:P4,,ReutersRtMode,,M5)</f>
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
       </c>
       <c r="M4" s="142" t="s">
         <v>157</v>
@@ -13225,9 +13225,9 @@
       <c r="U8" s="156">
         <v>0.06</v>
       </c>
-      <c r="V8" s="94" t="e">
+      <c r="V8" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E8,$U8/100,ISERROR(F8))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W8" s="84"/>
       <c r="X8" s="281"/>
@@ -13287,9 +13287,9 @@
       <c r="U9" s="156">
         <v>0.06</v>
       </c>
-      <c r="V9" s="94" t="e">
+      <c r="V9" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E9,$U9/100,ISERROR(F9))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W9" s="84"/>
       <c r="X9" s="281"/>
@@ -13349,9 +13349,9 @@
       <c r="U10" s="156">
         <v>6.9999999999999993E-2</v>
       </c>
-      <c r="V10" s="94" t="e">
+      <c r="V10" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E10,$U10/100,ISERROR(F10))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W10" s="84"/>
       <c r="X10" s="281"/>
@@ -13411,9 +13411,9 @@
       <c r="U11" s="156">
         <v>0.1</v>
       </c>
-      <c r="V11" s="94" t="e">
+      <c r="V11" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E11,$U11/100,ISERROR(F11))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W11" s="84"/>
       <c r="X11" s="281"/>
@@ -13473,9 +13473,9 @@
       <c r="U12" s="156">
         <v>0.11</v>
       </c>
-      <c r="V12" s="94" t="e">
+      <c r="V12" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E12,$U12/100,ISERROR(F12))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W12" s="84"/>
       <c r="X12" s="281"/>
@@ -13535,9 +13535,9 @@
       <c r="U13" s="156">
         <v>0.12000000000000001</v>
       </c>
-      <c r="V13" s="94" t="e">
+      <c r="V13" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E13,$U13/100,ISERROR(F13))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W13" s="84"/>
       <c r="X13" s="281"/>
@@ -13721,9 +13721,9 @@
       <c r="U16" s="156">
         <v>0.13</v>
       </c>
-      <c r="V16" s="94" t="e">
+      <c r="V16" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E16,$U16/100,ISERROR(F16))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W16" s="84"/>
       <c r="X16" s="281"/>
@@ -13907,9 +13907,9 @@
       <c r="U19" s="156">
         <v>0.15000000000000002</v>
       </c>
-      <c r="V19" s="94" t="e">
+      <c r="V19" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E19,$U19/100,ISERROR(F19))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W19" s="84"/>
       <c r="X19" s="281"/>
@@ -14320,7 +14320,7 @@
       <c r="N2" s="108"/>
       <c r="O2" s="107">
         <f>_xll.ohTrigger(O4:O21)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="P2" s="84"/>
     </row>
@@ -14345,7 +14345,7 @@
       <c r="H3" s="93"/>
       <c r="I3" s="214" t="str">
         <f>_xll.RData(I4:I21,J3:J3,,ReutersRtMode,,J4)</f>
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:20</v>
       </c>
       <c r="J3" s="105" t="s">
         <v>138</v>
@@ -14387,24 +14387,24 @@
         <v>HIHKDOND=</v>
       </c>
       <c r="J4" s="101">
-        <v>4.7990000000000005E-2</v>
+        <v>5.6530000000000004E-2</v>
       </c>
       <c r="K4" s="88" t="s">
         <v>177</v>
       </c>
       <c r="L4" s="100">
-        <v>4.7990000000000005E-2</v>
+        <v>5.6530000000000004E-2</v>
       </c>
       <c r="M4" s="88" t="s">
         <v>177</v>
       </c>
       <c r="N4" s="167">
         <f t="array" ref="N4:N21">QuoteLive</f>
-        <v>4.7990000000000005E-2</v>
-      </c>
-      <c r="O4" s="98" t="e">
+        <v>5.6530000000000004E-2</v>
+      </c>
+      <c r="O4" s="98">
         <f>_xll.qlSimpleQuoteSetValue(C4,N4/100,ISERROR(D4))</f>
-        <v>#N/A</v>
+        <v>8.5399999999999962E-5</v>
       </c>
       <c r="P4" s="84"/>
     </row>
@@ -14564,23 +14564,23 @@
         <v>HIHKD2WD=</v>
       </c>
       <c r="J8" s="90">
-        <v>0.13820000000000002</v>
+        <v>0.16257000000000002</v>
       </c>
       <c r="K8" s="88" t="s">
         <v>177</v>
       </c>
       <c r="L8" s="97">
-        <v>0.13820000000000002</v>
+        <v>0.16257000000000002</v>
       </c>
       <c r="M8" s="88" t="s">
         <v>177</v>
       </c>
       <c r="N8" s="156">
-        <v>0.13820000000000002</v>
-      </c>
-      <c r="O8" s="94" t="e">
+        <v>0.16257000000000002</v>
+      </c>
+      <c r="O8" s="94">
         <f>_xll.qlSimpleQuoteSetValue(C8,N8/100,ISERROR(D8))</f>
-        <v>#N/A</v>
+        <v>2.4369999999999991E-4</v>
       </c>
       <c r="P8" s="84"/>
     </row>
@@ -14652,23 +14652,23 @@
         <v>HIHKD1MD=</v>
       </c>
       <c r="J10" s="90">
-        <v>0.24043000000000003</v>
+        <v>0.24094000000000002</v>
       </c>
       <c r="K10" s="88" t="s">
         <v>177</v>
       </c>
       <c r="L10" s="97">
-        <v>0.24043000000000003</v>
+        <v>0.24094000000000002</v>
       </c>
       <c r="M10" s="88" t="s">
         <v>177</v>
       </c>
       <c r="N10" s="156">
-        <v>0.24043000000000003</v>
-      </c>
-      <c r="O10" s="94" t="e">
+        <v>0.24094000000000002</v>
+      </c>
+      <c r="O10" s="94">
         <f>_xll.qlSimpleQuoteSetValue(C10,N10/100,ISERROR(D10))</f>
-        <v>#N/A</v>
+        <v>5.1000000000000698E-6</v>
       </c>
       <c r="P10" s="84"/>
     </row>
@@ -14696,23 +14696,23 @@
         <v>HIHKD2MD=</v>
       </c>
       <c r="J11" s="90">
-        <v>0.30371000000000004</v>
+        <v>0.30586000000000002</v>
       </c>
       <c r="K11" s="88" t="s">
         <v>177</v>
       </c>
       <c r="L11" s="97">
-        <v>0.30371000000000004</v>
+        <v>0.30586000000000002</v>
       </c>
       <c r="M11" s="88" t="s">
         <v>177</v>
       </c>
       <c r="N11" s="156">
-        <v>0.30371000000000004</v>
-      </c>
-      <c r="O11" s="94" t="e">
+        <v>0.30586000000000002</v>
+      </c>
+      <c r="O11" s="94">
         <f>_xll.qlSimpleQuoteSetValue(C11,N11/100,ISERROR(D11))</f>
-        <v>#N/A</v>
+        <v>2.1499999999999818E-5</v>
       </c>
       <c r="P11" s="84"/>
     </row>
@@ -14740,23 +14740,23 @@
         <v>HIHKD3MD=</v>
       </c>
       <c r="J12" s="90">
-        <v>0.38600000000000001</v>
+        <v>0.38814000000000004</v>
       </c>
       <c r="K12" s="88" t="s">
         <v>177</v>
       </c>
       <c r="L12" s="97">
-        <v>0.38600000000000001</v>
+        <v>0.38814000000000004</v>
       </c>
       <c r="M12" s="88" t="s">
         <v>177</v>
       </c>
       <c r="N12" s="156">
-        <v>0.38600000000000001</v>
-      </c>
-      <c r="O12" s="94" t="e">
+        <v>0.38814000000000004</v>
+      </c>
+      <c r="O12" s="94">
         <f>_xll.qlSimpleQuoteSetValue(C12,N12/100,ISERROR(D12))</f>
-        <v>#N/A</v>
+        <v>2.1400000000000412E-5</v>
       </c>
       <c r="P12" s="84"/>
     </row>
@@ -14872,23 +14872,23 @@
         <v>HIHKD6MD=</v>
       </c>
       <c r="J15" s="90">
-        <v>0.54136000000000006</v>
+        <v>0.54286000000000001</v>
       </c>
       <c r="K15" s="88" t="s">
         <v>177</v>
       </c>
       <c r="L15" s="97">
-        <v>0.54136000000000006</v>
+        <v>0.54286000000000001</v>
       </c>
       <c r="M15" s="88" t="s">
         <v>177</v>
       </c>
       <c r="N15" s="156">
-        <v>0.54136000000000006</v>
-      </c>
-      <c r="O15" s="94" t="e">
+        <v>0.54286000000000001</v>
+      </c>
+      <c r="O15" s="94">
         <f>_xll.qlSimpleQuoteSetValue(C15,N15/100,ISERROR(D15))</f>
-        <v>#N/A</v>
+        <v>1.4999999999999389E-5</v>
       </c>
       <c r="P15" s="84"/>
     </row>
@@ -15136,23 +15136,23 @@
         <v>HIHKD1YD=</v>
       </c>
       <c r="J21" s="90">
-        <v>0.84153000000000011</v>
+        <v>0.8432900000000001</v>
       </c>
       <c r="K21" s="88" t="s">
         <v>177</v>
       </c>
       <c r="L21" s="89">
-        <v>0.84153000000000011</v>
+        <v>0.8432900000000001</v>
       </c>
       <c r="M21" s="88" t="s">
         <v>177</v>
       </c>
       <c r="N21" s="149">
-        <v>0.84153000000000011</v>
-      </c>
-      <c r="O21" s="85" t="e">
+        <v>0.8432900000000001</v>
+      </c>
+      <c r="O21" s="85">
         <f>_xll.qlSimpleQuoteSetValue(C21,N21/100,ISERROR(D21))</f>
-        <v>#N/A</v>
+        <v>1.759999999999956E-5</v>
       </c>
       <c r="P21" s="84"/>
     </row>
@@ -15295,7 +15295,7 @@
       <c r="V3" s="146"/>
       <c r="W3" s="107">
         <f>_xll.ohTrigger(W7:W28)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="X3" s="109"/>
       <c r="Y3" s="116"/>
@@ -15327,7 +15327,7 @@
       <c r="L4" s="143"/>
       <c r="M4" s="106" t="str">
         <f>_xll.RData(M7:M38,N4:Q4,,ReutersRtMode,,N7)</f>
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
       </c>
       <c r="N4" s="142" t="s">
         <v>157</v>
@@ -15639,9 +15639,9 @@
       <c r="V9" s="156">
         <v>0.41000000000000003</v>
       </c>
-      <c r="W9" s="94" t="e">
+      <c r="W9" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D9,V9/100,ISERROR(E9))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="X9" s="84"/>
       <c r="Y9" s="116"/>
@@ -15707,9 +15707,9 @@
       <c r="V10" s="156">
         <v>0.41000000000000003</v>
       </c>
-      <c r="W10" s="94" t="e">
+      <c r="W10" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D10,V10/100,ISERROR(E10))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="X10" s="84"/>
       <c r="Y10" s="116"/>
@@ -15752,10 +15752,10 @@
         <v>HKD3X6F=PREA</v>
       </c>
       <c r="N11" s="127">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="O11" s="127">
-        <v>0.48</v>
+        <v>0.49</v>
       </c>
       <c r="P11" s="126">
         <v>0</v>
@@ -15765,19 +15765,19 @@
       </c>
       <c r="R11" s="90">
         <f>_xll.qlMidSafe($N11,$O11)</f>
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="S11" s="88"/>
       <c r="T11" s="125">
-        <v>0.43</v>
+        <v>0.44</v>
       </c>
       <c r="U11" s="88"/>
       <c r="V11" s="156">
-        <v>0.43</v>
-      </c>
-      <c r="W11" s="94" t="e">
+        <v>0.44</v>
+      </c>
+      <c r="W11" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D11,V11/100,ISERROR(E11))</f>
-        <v>#N/A</v>
+        <v>1.0000000000000026E-4</v>
       </c>
       <c r="X11" s="84"/>
       <c r="Y11" s="116"/>
@@ -15820,10 +15820,10 @@
         <v>HKD4X7F=PREA</v>
       </c>
       <c r="N12" s="127">
-        <v>0.41000000000000003</v>
+        <v>0.43</v>
       </c>
       <c r="O12" s="127">
-        <v>0.51</v>
+        <v>0.53</v>
       </c>
       <c r="P12" s="126">
         <v>0</v>
@@ -15833,19 +15833,19 @@
       </c>
       <c r="R12" s="90">
         <f>_xll.qlMidSafe($N12,$O12)</f>
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="S12" s="88"/>
       <c r="T12" s="125">
-        <v>0.46</v>
+        <v>0.48</v>
       </c>
       <c r="U12" s="88"/>
       <c r="V12" s="156">
-        <v>0.46</v>
-      </c>
-      <c r="W12" s="94" t="e">
+        <v>0.48</v>
+      </c>
+      <c r="W12" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D12,V12/100,ISERROR(E12))</f>
-        <v>#N/A</v>
+        <v>1.9999999999999966E-4</v>
       </c>
       <c r="X12" s="84"/>
       <c r="Y12" s="116"/>
@@ -15888,10 +15888,10 @@
         <v>HKD5X8F=PREA</v>
       </c>
       <c r="N13" s="127">
-        <v>0.44</v>
+        <v>0.48</v>
       </c>
       <c r="O13" s="127">
-        <v>0.54</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="P13" s="126">
         <v>0</v>
@@ -15901,19 +15901,19 @@
       </c>
       <c r="R13" s="90">
         <f>_xll.qlMidSafe($N13,$O13)</f>
-        <v>0.49</v>
+        <v>0.53</v>
       </c>
       <c r="S13" s="88"/>
       <c r="T13" s="125">
-        <v>0.49</v>
+        <v>0.53</v>
       </c>
       <c r="U13" s="88"/>
       <c r="V13" s="156">
-        <v>0.49</v>
-      </c>
-      <c r="W13" s="94" t="e">
+        <v>0.53</v>
+      </c>
+      <c r="W13" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D13,V13/100,ISERROR(E13))</f>
-        <v>#N/A</v>
+        <v>4.0000000000000018E-4</v>
       </c>
       <c r="X13" s="84"/>
       <c r="Y13" s="116"/>
@@ -15956,10 +15956,10 @@
         <v>HKD6X9F=PREA</v>
       </c>
       <c r="N14" s="127">
-        <v>0.46</v>
+        <v>0.52</v>
       </c>
       <c r="O14" s="127">
-        <v>0.56000000000000005</v>
+        <v>0.62</v>
       </c>
       <c r="P14" s="126">
         <v>0</v>
@@ -15969,19 +15969,19 @@
       </c>
       <c r="R14" s="90">
         <f>_xll.qlMidSafe($N14,$O14)</f>
-        <v>0.51</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="S14" s="88"/>
       <c r="T14" s="125">
-        <v>0.51</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="U14" s="88"/>
       <c r="V14" s="156">
-        <v>0.51</v>
-      </c>
-      <c r="W14" s="94" t="e">
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="W14" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D14,V14/100,ISERROR(E14))</f>
-        <v>#N/A</v>
+        <v>5.9999999999999984E-4</v>
       </c>
       <c r="X14" s="84"/>
       <c r="Y14" s="116"/>
@@ -16024,10 +16024,10 @@
         <v>HKD7X10F=PREA</v>
       </c>
       <c r="N15" s="127">
-        <v>0.5</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="O15" s="127">
-        <v>0.6</v>
+        <v>0.67</v>
       </c>
       <c r="P15" s="126">
         <v>0</v>
@@ -16037,19 +16037,19 @@
       </c>
       <c r="R15" s="90">
         <f>_xll.qlMidSafe($N15,$O15)</f>
-        <v>0.55000000000000004</v>
+        <v>0.62000000000000011</v>
       </c>
       <c r="S15" s="88"/>
       <c r="T15" s="125">
-        <v>0.55000000000000004</v>
+        <v>0.62000000000000011</v>
       </c>
       <c r="U15" s="88"/>
       <c r="V15" s="156">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="W15" s="94" t="e">
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="W15" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D15,V15/100,ISERROR(E15))</f>
-        <v>#N/A</v>
+        <v>7.000000000000001E-4</v>
       </c>
       <c r="X15" s="84"/>
       <c r="Y15" s="116"/>
@@ -16092,10 +16092,10 @@
         <v>HKD8X11F=PREA</v>
       </c>
       <c r="N16" s="127">
-        <v>0.55000000000000004</v>
+        <v>0.62</v>
       </c>
       <c r="O16" s="127">
-        <v>0.65</v>
+        <v>0.72</v>
       </c>
       <c r="P16" s="126">
         <v>0</v>
@@ -16105,19 +16105,19 @@
       </c>
       <c r="R16" s="90">
         <f>_xll.qlMidSafe($N16,$O16)</f>
-        <v>0.60000000000000009</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="S16" s="88"/>
       <c r="T16" s="125">
-        <v>0.60000000000000009</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="U16" s="88"/>
       <c r="V16" s="156">
-        <v>0.60000000000000009</v>
-      </c>
-      <c r="W16" s="94" t="e">
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="W16" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D16,V16/100,ISERROR(E16))</f>
-        <v>#N/A</v>
+        <v>6.9999999999999837E-4</v>
       </c>
       <c r="X16" s="84"/>
       <c r="Y16" s="116"/>
@@ -16160,10 +16160,10 @@
         <v>HKD9X12F=PREA</v>
       </c>
       <c r="N17" s="133">
-        <v>0.59</v>
+        <v>0.68</v>
       </c>
       <c r="O17" s="133">
-        <v>0.69000000000000006</v>
+        <v>0.78</v>
       </c>
       <c r="P17" s="132">
         <v>0</v>
@@ -16173,19 +16173,19 @@
       </c>
       <c r="R17" s="131">
         <f>_xll.qlMidSafe($N17,$O17)</f>
-        <v>0.64</v>
+        <v>0.73</v>
       </c>
       <c r="S17" s="88"/>
       <c r="T17" s="130">
-        <v>0.64</v>
+        <v>0.73</v>
       </c>
       <c r="U17" s="88"/>
       <c r="V17" s="156">
-        <v>0.64</v>
-      </c>
-      <c r="W17" s="94" t="e">
+        <v>0.73</v>
+      </c>
+      <c r="W17" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D17,V17/100,ISERROR(E17))</f>
-        <v>#N/A</v>
+        <v>8.9999999999999976E-4</v>
       </c>
       <c r="X17" s="84"/>
       <c r="Y17" s="116"/>
@@ -16366,10 +16366,10 @@
         <v>HKD1X7F=PREA</v>
       </c>
       <c r="N20" s="127">
-        <v>0.46</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="O20" s="127">
-        <v>0.56000000000000005</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="P20" s="126">
         <v>0</v>
@@ -16379,19 +16379,19 @@
       </c>
       <c r="R20" s="90">
         <f>_xll.qlMidSafe($N20,$O20)</f>
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="S20" s="88"/>
       <c r="T20" s="125">
-        <v>0.51</v>
+        <v>0.52</v>
       </c>
       <c r="U20" s="88"/>
       <c r="V20" s="156">
-        <v>0.51</v>
-      </c>
-      <c r="W20" s="94" t="e">
+        <v>0.52</v>
+      </c>
+      <c r="W20" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D20,V20/100,ISERROR(E20))</f>
-        <v>#N/A</v>
+        <v>9.9999999999999395E-5</v>
       </c>
       <c r="X20" s="84"/>
       <c r="Y20" s="116"/>
@@ -16436,10 +16436,10 @@
         <v>HKD2X8F=PREA</v>
       </c>
       <c r="N21" s="127">
-        <v>0.47000000000000003</v>
+        <v>0.49</v>
       </c>
       <c r="O21" s="127">
-        <v>0.57000000000000006</v>
+        <v>0.59</v>
       </c>
       <c r="P21" s="126">
         <v>0</v>
@@ -16449,19 +16449,19 @@
       </c>
       <c r="R21" s="90">
         <f>_xll.qlMidSafe($N21,$O21)</f>
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
       <c r="S21" s="88"/>
       <c r="T21" s="125">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
       <c r="U21" s="88"/>
       <c r="V21" s="156">
-        <v>0.52</v>
-      </c>
-      <c r="W21" s="94" t="e">
+        <v>0.54</v>
+      </c>
+      <c r="W21" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D21,V21/100,ISERROR(E21))</f>
-        <v>#N/A</v>
+        <v>2.0000000000000052E-4</v>
       </c>
       <c r="X21" s="84"/>
       <c r="Y21" s="116"/>
@@ -16506,10 +16506,10 @@
         <v>HKD3X9F=PREA</v>
       </c>
       <c r="N22" s="127">
-        <v>0.5</v>
+        <v>0.53</v>
       </c>
       <c r="O22" s="127">
-        <v>0.6</v>
+        <v>0.63</v>
       </c>
       <c r="P22" s="126">
         <v>0</v>
@@ -16519,19 +16519,19 @@
       </c>
       <c r="R22" s="90">
         <f>_xll.qlMidSafe($N22,$O22)</f>
-        <v>0.55000000000000004</v>
+        <v>0.58000000000000007</v>
       </c>
       <c r="S22" s="88"/>
       <c r="T22" s="125">
-        <v>0.55000000000000004</v>
+        <v>0.58000000000000007</v>
       </c>
       <c r="U22" s="88"/>
       <c r="V22" s="156">
-        <v>0.55000000000000004</v>
-      </c>
-      <c r="W22" s="94" t="e">
+        <v>0.58000000000000007</v>
+      </c>
+      <c r="W22" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D22,V22/100,ISERROR(E22))</f>
-        <v>#N/A</v>
+        <v>2.9999999999999992E-4</v>
       </c>
       <c r="X22" s="84"/>
       <c r="Y22" s="116"/>
@@ -16576,10 +16576,10 @@
         <v>HKD4X10F=PREA</v>
       </c>
       <c r="N23" s="127">
-        <v>0.53</v>
+        <v>0.57000000000000006</v>
       </c>
       <c r="O23" s="127">
-        <v>0.63</v>
+        <v>0.67</v>
       </c>
       <c r="P23" s="126">
         <v>0</v>
@@ -16589,19 +16589,19 @@
       </c>
       <c r="R23" s="90">
         <f>_xll.qlMidSafe($N23,$O23)</f>
-        <v>0.58000000000000007</v>
+        <v>0.62000000000000011</v>
       </c>
       <c r="S23" s="88"/>
       <c r="T23" s="125">
-        <v>0.58000000000000007</v>
+        <v>0.62000000000000011</v>
       </c>
       <c r="U23" s="88"/>
       <c r="V23" s="156">
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="W23" s="94" t="e">
+        <v>0.62000000000000011</v>
+      </c>
+      <c r="W23" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D23,V23/100,ISERROR(E23))</f>
-        <v>#N/A</v>
+        <v>4.0000000000000018E-4</v>
       </c>
       <c r="X23" s="84"/>
       <c r="Y23" s="116"/>
@@ -16646,10 +16646,10 @@
         <v>HKD5X11F=PREA</v>
       </c>
       <c r="N24" s="127">
-        <v>0.57000000000000006</v>
+        <v>0.62</v>
       </c>
       <c r="O24" s="127">
-        <v>0.67</v>
+        <v>0.72</v>
       </c>
       <c r="P24" s="126">
         <v>0</v>
@@ -16659,19 +16659,19 @@
       </c>
       <c r="R24" s="90">
         <f>_xll.qlMidSafe($N24,$O24)</f>
-        <v>0.62000000000000011</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="S24" s="88"/>
       <c r="T24" s="125">
-        <v>0.62000000000000011</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="U24" s="88"/>
       <c r="V24" s="156">
-        <v>0.62000000000000011</v>
-      </c>
-      <c r="W24" s="94" t="e">
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="W24" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D24,V24/100,ISERROR(E24))</f>
-        <v>#N/A</v>
+        <v>4.9999999999999871E-4</v>
       </c>
       <c r="X24" s="84"/>
       <c r="Y24" s="116"/>
@@ -16716,10 +16716,10 @@
         <v>HKD6X12F=PREA</v>
       </c>
       <c r="N25" s="127">
-        <v>0.61</v>
+        <v>0.67</v>
       </c>
       <c r="O25" s="127">
-        <v>0.71</v>
+        <v>0.77</v>
       </c>
       <c r="P25" s="126">
         <v>0</v>
@@ -16729,19 +16729,19 @@
       </c>
       <c r="R25" s="90">
         <f>_xll.qlMidSafe($N25,$O25)</f>
-        <v>0.65999999999999992</v>
+        <v>0.72</v>
       </c>
       <c r="S25" s="88"/>
       <c r="T25" s="125">
-        <v>0.65999999999999992</v>
+        <v>0.72</v>
       </c>
       <c r="U25" s="88"/>
       <c r="V25" s="156">
-        <v>0.65999999999999992</v>
-      </c>
-      <c r="W25" s="94" t="e">
+        <v>0.72</v>
+      </c>
+      <c r="W25" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D25,V25/100,ISERROR(E25))</f>
-        <v>#N/A</v>
+        <v>6.0000000000000071E-4</v>
       </c>
       <c r="X25" s="84"/>
       <c r="Y25" s="116"/>
@@ -17136,10 +17136,10 @@
         <v>HKD12X18F=PREA</v>
       </c>
       <c r="N31" s="127">
-        <v>1.02</v>
+        <v>0.98</v>
       </c>
       <c r="O31" s="127">
-        <v>1.1200000000000001</v>
+        <v>1.08</v>
       </c>
       <c r="P31" s="126">
         <v>0</v>
@@ -17149,19 +17149,19 @@
       </c>
       <c r="R31" s="90">
         <f>_xll.qlMidSafe($N31,$O31)</f>
-        <v>1.07</v>
+        <v>1.03</v>
       </c>
       <c r="S31" s="88"/>
       <c r="T31" s="125">
-        <v>1.07</v>
+        <v>1.03</v>
       </c>
       <c r="U31" s="88"/>
       <c r="V31" s="156">
-        <v>1.07</v>
-      </c>
-      <c r="W31" s="94" t="e">
+        <v>1.03</v>
+      </c>
+      <c r="W31" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D31,V31/100,ISERROR(E31))</f>
-        <v>#N/A</v>
+        <v>-4.0000000000000105E-4</v>
       </c>
       <c r="X31" s="84"/>
       <c r="Y31" s="116"/>
@@ -17556,10 +17556,10 @@
         <v>HKD18X24F=PREA</v>
       </c>
       <c r="N37" s="127">
-        <v>1.41</v>
+        <v>1.33</v>
       </c>
       <c r="O37" s="127">
-        <v>1.51</v>
+        <v>1.43</v>
       </c>
       <c r="P37" s="126">
         <v>0</v>
@@ -17569,19 +17569,19 @@
       </c>
       <c r="R37" s="90">
         <f>_xll.qlMidSafe($N37,$O37)</f>
-        <v>1.46</v>
+        <v>1.38</v>
       </c>
       <c r="S37" s="88"/>
       <c r="T37" s="125">
-        <v>1.46</v>
+        <v>1.38</v>
       </c>
       <c r="U37" s="88"/>
       <c r="V37" s="156">
-        <v>1.46</v>
-      </c>
-      <c r="W37" s="94" t="e">
+        <v>1.38</v>
+      </c>
+      <c r="W37" s="94">
         <f>_xll.qlSimpleQuoteSetValue(D37,V37/100,ISERROR(E37))</f>
-        <v>#N/A</v>
+        <v>-8.0000000000000036E-4</v>
       </c>
       <c r="X37" s="84"/>
       <c r="Y37" s="116"/>
@@ -18160,7 +18160,7 @@
       <c r="Y2" s="146"/>
       <c r="Z2" s="107">
         <f>_xll.ohTrigger(Z4:Z39)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="AA2" s="173"/>
       <c r="AB2" s="116"/>
@@ -18208,7 +18208,7 @@
       </c>
       <c r="O3" s="180" t="str">
         <f>_xll.RData(O4:O39,P3:T3,,ReutersRtMode,,P4)</f>
-        <v>Paused at 11:12:45</v>
+        <v>Updated at 14:24:19</v>
       </c>
       <c r="P3" s="177" t="s">
         <v>158</v>
@@ -18289,36 +18289,36 @@
         <v>HIRN5</v>
       </c>
       <c r="P4" s="169">
-        <v>42142</v>
+        <v>42198</v>
       </c>
       <c r="Q4" s="99">
-        <v>99.54</v>
+        <v>99.53</v>
       </c>
       <c r="R4" s="99">
-        <v>99.64</v>
+        <v>99.63</v>
       </c>
       <c r="S4" s="99">
         <v>0</v>
       </c>
       <c r="T4" s="99">
-        <v>99.59</v>
+        <v>99.58</v>
       </c>
       <c r="U4" s="101">
         <f>_xll.qlMidSafe($Q4,$R4)</f>
-        <v>99.59</v>
+        <v>99.58</v>
       </c>
       <c r="V4" s="88"/>
       <c r="W4" s="168">
-        <v>99.59</v>
+        <v>99.58</v>
       </c>
       <c r="X4" s="88"/>
       <c r="Y4" s="167">
         <f t="array" ref="Y4:Y39">QuoteLive</f>
-        <v>99.59</v>
-      </c>
-      <c r="Z4" s="101" t="e">
+        <v>99.58</v>
+      </c>
+      <c r="Z4" s="101">
         <f>_xll.qlSimpleQuoteSetValue(E4,$Y4,ISERROR(F4))</f>
-        <v>#N/A</v>
+        <v>-1.0000000000005116E-2</v>
       </c>
       <c r="AA4" s="109"/>
       <c r="AB4" s="116"/>
@@ -18367,35 +18367,35 @@
         <v>HIRQ5</v>
       </c>
       <c r="P5" s="158">
-        <v>42170</v>
+        <v>42233</v>
       </c>
       <c r="Q5" s="95">
-        <v>99.54</v>
+        <v>99.53</v>
       </c>
       <c r="R5" s="95">
-        <v>99.64</v>
+        <v>99.63</v>
       </c>
       <c r="S5" s="95">
         <v>0</v>
       </c>
       <c r="T5" s="95">
-        <v>99.59</v>
+        <v>99.58</v>
       </c>
       <c r="U5" s="90">
         <f>_xll.qlMidSafe($Q5,$R5)</f>
-        <v>99.59</v>
+        <v>99.58</v>
       </c>
       <c r="V5" s="88"/>
       <c r="W5" s="166">
-        <v>99.59</v>
+        <v>99.58</v>
       </c>
       <c r="X5" s="88"/>
       <c r="Y5" s="156">
-        <v>99.59</v>
-      </c>
-      <c r="Z5" s="90" t="e">
+        <v>99.58</v>
+      </c>
+      <c r="Z5" s="90">
         <f>_xll.qlSimpleQuoteSetValue(E5,$Y5,ISERROR(F5))</f>
-        <v>#N/A</v>
+        <v>-1.0000000000005116E-2</v>
       </c>
       <c r="AA5" s="109"/>
       <c r="AB5" s="116"/>
@@ -18444,35 +18444,35 @@
         <v>HIRU5</v>
       </c>
       <c r="P6" s="158">
-        <v>42198</v>
+        <v>42261</v>
       </c>
       <c r="Q6" s="95">
-        <v>99.54</v>
+        <v>99.53</v>
       </c>
       <c r="R6" s="95">
-        <v>99.64</v>
+        <v>99.63</v>
       </c>
       <c r="S6" s="95">
         <v>0</v>
       </c>
       <c r="T6" s="95">
-        <v>99.59</v>
+        <v>99.56</v>
       </c>
       <c r="U6" s="90">
         <f>_xll.qlMidSafe($Q6,$R6)</f>
-        <v>99.59</v>
+        <v>99.58</v>
       </c>
       <c r="V6" s="88"/>
       <c r="W6" s="166">
-        <v>99.59</v>
+        <v>99.58</v>
       </c>
       <c r="X6" s="88"/>
       <c r="Y6" s="156">
-        <v>99.59</v>
-      </c>
-      <c r="Z6" s="90" t="e">
+        <v>99.58</v>
+      </c>
+      <c r="Z6" s="90">
         <f>_xll.qlSimpleQuoteSetValue(E6,$Y6,ISERROR(F6))</f>
-        <v>#N/A</v>
+        <v>-1.0000000000005116E-2</v>
       </c>
       <c r="AA6" s="109"/>
       <c r="AB6" s="116"/>
@@ -18597,32 +18597,32 @@
         <f t="shared" si="1"/>
         <v>HIRX5</v>
       </c>
-      <c r="P8" s="158">
-        <v>42261</v>
-      </c>
-      <c r="Q8" s="95">
-        <v>99.5</v>
-      </c>
-      <c r="R8" s="95">
-        <v>99.600000000000009</v>
-      </c>
-      <c r="S8" s="95">
-        <v>0</v>
-      </c>
-      <c r="T8" s="95">
-        <v>99.55</v>
-      </c>
-      <c r="U8" s="90">
+      <c r="P8" s="158" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q8" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="R8" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="S8" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="T8" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="U8" s="90" t="e">
         <f>_xll.qlMidSafe($Q8,$R8)</f>
-        <v>99.550000000000011</v>
+        <v>#NUM!</v>
       </c>
       <c r="V8" s="88"/>
-      <c r="W8" s="157">
-        <v>99.550000000000011</v>
+      <c r="W8" s="157" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X8" s="88"/>
-      <c r="Y8" s="156">
-        <v>99.550000000000011</v>
+      <c r="Y8" s="156" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="Z8" s="90" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E8,$Y8,ISERROR(F8))</f>
@@ -18674,36 +18674,36 @@
         <f t="shared" si="1"/>
         <v>HIRZ5</v>
       </c>
-      <c r="P9" s="158" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q9" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="R9" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="S9" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="T9" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="U9" s="90" t="e">
+      <c r="P9" s="158">
+        <v>42352</v>
+      </c>
+      <c r="Q9" s="95">
+        <v>99.4</v>
+      </c>
+      <c r="R9" s="95">
+        <v>99.5</v>
+      </c>
+      <c r="S9" s="95">
+        <v>0</v>
+      </c>
+      <c r="T9" s="95">
+        <v>99.45</v>
+      </c>
+      <c r="U9" s="90">
         <f>_xll.qlMidSafe($Q9,$R9)</f>
-        <v>#NUM!</v>
+        <v>99.45</v>
       </c>
       <c r="V9" s="88"/>
-      <c r="W9" s="157" t="e">
-        <v>#NUM!</v>
+      <c r="W9" s="157">
+        <v>99.45</v>
       </c>
       <c r="X9" s="88"/>
-      <c r="Y9" s="156" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Z9" s="90">
+      <c r="Y9" s="156">
+        <v>99.45</v>
+      </c>
+      <c r="Z9" s="90" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E9,$Y9,ISERROR(F9))</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA9" s="109"/>
       <c r="AB9" s="116"/>
@@ -18828,32 +18828,32 @@
         <f t="shared" si="1"/>
         <v>HIRG6</v>
       </c>
-      <c r="P11" s="158">
-        <v>42352</v>
-      </c>
-      <c r="Q11" s="95">
-        <v>99.4</v>
-      </c>
-      <c r="R11" s="95">
-        <v>99.5</v>
-      </c>
-      <c r="S11" s="95">
-        <v>0</v>
-      </c>
-      <c r="T11" s="95">
-        <v>99.45</v>
-      </c>
-      <c r="U11" s="90">
+      <c r="P11" s="158" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q11" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="R11" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="S11" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="T11" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="U11" s="90" t="e">
         <f>_xll.qlMidSafe($Q11,$R11)</f>
-        <v>99.45</v>
+        <v>#NUM!</v>
       </c>
       <c r="V11" s="88"/>
-      <c r="W11" s="157">
-        <v>99.45</v>
+      <c r="W11" s="157" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X11" s="88"/>
-      <c r="Y11" s="156">
-        <v>99.45</v>
+      <c r="Y11" s="156" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="Z11" s="90" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E11,$Y11,ISERROR(F11))</f>
@@ -18905,36 +18905,36 @@
         <f t="shared" si="1"/>
         <v>HIRH6</v>
       </c>
-      <c r="P12" s="158" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q12" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="R12" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="S12" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="T12" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="U12" s="90" t="e">
+      <c r="P12" s="158">
+        <v>42443</v>
+      </c>
+      <c r="Q12" s="95">
+        <v>99.25</v>
+      </c>
+      <c r="R12" s="95">
+        <v>99.350000000000009</v>
+      </c>
+      <c r="S12" s="95">
+        <v>0</v>
+      </c>
+      <c r="T12" s="95">
+        <v>99.3</v>
+      </c>
+      <c r="U12" s="90">
         <f>_xll.qlMidSafe($Q12,$R12)</f>
-        <v>#NUM!</v>
+        <v>99.300000000000011</v>
       </c>
       <c r="V12" s="88"/>
-      <c r="W12" s="157" t="e">
-        <v>#NUM!</v>
+      <c r="W12" s="157">
+        <v>99.300000000000011</v>
       </c>
       <c r="X12" s="88"/>
-      <c r="Y12" s="156" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Z12" s="90">
+      <c r="Y12" s="156">
+        <v>99.300000000000011</v>
+      </c>
+      <c r="Z12" s="90" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E12,$Y12,ISERROR(F12))</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA12" s="109"/>
       <c r="AB12" s="116"/>
@@ -19059,32 +19059,32 @@
         <f t="shared" si="1"/>
         <v>HIRK6</v>
       </c>
-      <c r="P14" s="158">
-        <v>42443</v>
-      </c>
-      <c r="Q14" s="95">
-        <v>99.2</v>
-      </c>
-      <c r="R14" s="95">
-        <v>99.3</v>
-      </c>
-      <c r="S14" s="95">
-        <v>0</v>
-      </c>
-      <c r="T14" s="95">
-        <v>99.210000000000008</v>
-      </c>
-      <c r="U14" s="90">
+      <c r="P14" s="158" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q14" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="R14" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="S14" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="T14" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="U14" s="90" t="e">
         <f>_xll.qlMidSafe($Q14,$R14)</f>
-        <v>99.25</v>
+        <v>#NUM!</v>
       </c>
       <c r="V14" s="88"/>
-      <c r="W14" s="157">
-        <v>99.25</v>
+      <c r="W14" s="157" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="X14" s="88"/>
-      <c r="Y14" s="156">
-        <v>99.25</v>
+      <c r="Y14" s="156" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="Z14" s="90" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E14,$Y14,ISERROR(F14))</f>
@@ -19136,36 +19136,36 @@
         <f t="shared" si="1"/>
         <v>HIRM6</v>
       </c>
-      <c r="P15" s="158" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q15" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="R15" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="S15" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="T15" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="U15" s="90" t="e">
+      <c r="P15" s="158">
+        <v>42534</v>
+      </c>
+      <c r="Q15" s="95">
+        <v>99.100000000000009</v>
+      </c>
+      <c r="R15" s="95">
+        <v>99.2</v>
+      </c>
+      <c r="S15" s="95">
+        <v>0</v>
+      </c>
+      <c r="T15" s="95">
+        <v>99.11</v>
+      </c>
+      <c r="U15" s="90">
         <f>_xll.qlMidSafe($Q15,$R15)</f>
-        <v>#NUM!</v>
+        <v>99.15</v>
       </c>
       <c r="V15" s="88"/>
-      <c r="W15" s="157" t="e">
-        <v>#NUM!</v>
+      <c r="W15" s="157">
+        <v>99.15</v>
       </c>
       <c r="X15" s="88"/>
-      <c r="Y15" s="156" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="Z15" s="90">
+      <c r="Y15" s="156">
+        <v>99.15</v>
+      </c>
+      <c r="Z15" s="90" t="e">
         <f>_xll.qlSimpleQuoteSetValue(E15,$Y15,ISERROR(F15))</f>
-        <v>0</v>
+        <v>#N/A</v>
       </c>
       <c r="AA15" s="109"/>
       <c r="AB15" s="116"/>
@@ -19290,20 +19290,20 @@
         <f t="shared" si="1"/>
         <v>HIRQ6</v>
       </c>
-      <c r="P17" s="158">
-        <v>42534</v>
-      </c>
-      <c r="Q17" s="95">
-        <v>0</v>
-      </c>
-      <c r="R17" s="95">
-        <v>0</v>
-      </c>
-      <c r="S17" s="95">
-        <v>0</v>
-      </c>
-      <c r="T17" s="95">
-        <v>99.210000000000008</v>
+      <c r="P17" s="158" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q17" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="R17" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="S17" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="T17" s="95" t="s">
+        <v>204</v>
       </c>
       <c r="U17" s="90" t="e">
         <f>_xll.qlMidSafe($Q17,$R17)</f>
@@ -19367,20 +19367,20 @@
         <f t="shared" si="1"/>
         <v>HIRU6</v>
       </c>
-      <c r="P18" s="158" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q18" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="R18" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="S18" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="T18" s="95" t="s">
-        <v>204</v>
+      <c r="P18" s="158">
+        <v>42632</v>
+      </c>
+      <c r="Q18" s="95">
+        <v>0</v>
+      </c>
+      <c r="R18" s="95">
+        <v>0</v>
+      </c>
+      <c r="S18" s="95">
+        <v>0</v>
+      </c>
+      <c r="T18" s="95">
+        <v>99.11</v>
       </c>
       <c r="U18" s="90" t="e">
         <f>_xll.qlMidSafe($Q18,$R18)</f>
@@ -19521,20 +19521,20 @@
         <f t="shared" si="1"/>
         <v>HIRX6</v>
       </c>
-      <c r="P20" s="158">
-        <v>42632</v>
-      </c>
-      <c r="Q20" s="95">
-        <v>0</v>
-      </c>
-      <c r="R20" s="95">
-        <v>0</v>
-      </c>
-      <c r="S20" s="95">
-        <v>0</v>
-      </c>
-      <c r="T20" s="95">
-        <v>99.210000000000008</v>
+      <c r="P20" s="158" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q20" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="R20" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="S20" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="T20" s="95" t="s">
+        <v>204</v>
       </c>
       <c r="U20" s="90" t="e">
         <f>_xll.qlMidSafe($Q20,$R20)</f>
@@ -19598,20 +19598,20 @@
         <f t="shared" si="1"/>
         <v>HIRZ6</v>
       </c>
-      <c r="P21" s="158" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q21" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="R21" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="S21" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="T21" s="95" t="s">
-        <v>204</v>
+      <c r="P21" s="158">
+        <v>42723</v>
+      </c>
+      <c r="Q21" s="95">
+        <v>0</v>
+      </c>
+      <c r="R21" s="95">
+        <v>0</v>
+      </c>
+      <c r="S21" s="95">
+        <v>0</v>
+      </c>
+      <c r="T21" s="95">
+        <v>99.11</v>
       </c>
       <c r="U21" s="90" t="e">
         <f>_xll.qlMidSafe($Q21,$R21)</f>
@@ -19752,20 +19752,20 @@
         <f t="shared" si="1"/>
         <v>HIRG7</v>
       </c>
-      <c r="P23" s="158">
-        <v>42723</v>
-      </c>
-      <c r="Q23" s="95">
-        <v>0</v>
-      </c>
-      <c r="R23" s="95">
-        <v>0</v>
-      </c>
-      <c r="S23" s="95">
-        <v>0</v>
-      </c>
-      <c r="T23" s="95">
-        <v>99.210000000000008</v>
+      <c r="P23" s="158" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q23" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="R23" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="S23" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="T23" s="95" t="s">
+        <v>204</v>
       </c>
       <c r="U23" s="90" t="e">
         <f>_xll.qlMidSafe($Q23,$R23)</f>
@@ -19829,20 +19829,20 @@
         <f t="shared" si="1"/>
         <v>HIRH7</v>
       </c>
-      <c r="P24" s="158" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q24" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="R24" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="S24" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="T24" s="95" t="s">
-        <v>204</v>
+      <c r="P24" s="158">
+        <v>42807</v>
+      </c>
+      <c r="Q24" s="95">
+        <v>0</v>
+      </c>
+      <c r="R24" s="95">
+        <v>0</v>
+      </c>
+      <c r="S24" s="95">
+        <v>0</v>
+      </c>
+      <c r="T24" s="95">
+        <v>99.11</v>
       </c>
       <c r="U24" s="90" t="e">
         <f>_xll.qlMidSafe($Q24,$R24)</f>
@@ -19983,20 +19983,20 @@
         <f t="shared" si="1"/>
         <v>HIRK7</v>
       </c>
-      <c r="P26" s="158">
-        <v>42807</v>
-      </c>
-      <c r="Q26" s="95">
-        <v>0</v>
-      </c>
-      <c r="R26" s="95">
-        <v>0</v>
-      </c>
-      <c r="S26" s="95">
-        <v>0</v>
-      </c>
-      <c r="T26" s="95">
-        <v>99.210000000000008</v>
+      <c r="P26" s="158" t="s">
+        <v>204</v>
+      </c>
+      <c r="Q26" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="R26" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="S26" s="95" t="s">
+        <v>204</v>
+      </c>
+      <c r="T26" s="95" t="s">
+        <v>204</v>
       </c>
       <c r="U26" s="90" t="e">
         <f>_xll.qlMidSafe($Q26,$R26)</f>
@@ -20060,20 +20060,20 @@
         <f t="shared" si="1"/>
         <v>HIRM7</v>
       </c>
-      <c r="P27" s="158" t="s">
-        <v>204</v>
-      </c>
-      <c r="Q27" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="R27" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="S27" s="95" t="s">
-        <v>204</v>
-      </c>
-      <c r="T27" s="95" t="s">
-        <v>204</v>
+      <c r="P27" s="158">
+        <v>42905</v>
+      </c>
+      <c r="Q27" s="95">
+        <v>0</v>
+      </c>
+      <c r="R27" s="95">
+        <v>0</v>
+      </c>
+      <c r="S27" s="95">
+        <v>0</v>
+      </c>
+      <c r="T27" s="95">
+        <v>99.11</v>
       </c>
       <c r="U27" s="90" t="e">
         <f>_xll.qlMidSafe($Q27,$R27)</f>
@@ -21177,7 +21177,7 @@
       <c r="U3" s="146"/>
       <c r="V3" s="107">
         <f>_xll.ohTrigger(V5:V15)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="W3" s="84"/>
       <c r="X3" s="281"/>
@@ -21208,7 +21208,7 @@
       <c r="K4" s="145"/>
       <c r="L4" s="106" t="str">
         <f>_xll.RData(L5:L15,M4:P4,,ReutersRtMode,,M5)</f>
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
       </c>
       <c r="M4" s="142" t="s">
         <v>157</v>
@@ -21364,9 +21364,9 @@
       <c r="U6" s="156">
         <v>0.21000000000000002</v>
       </c>
-      <c r="V6" s="94" t="e">
+      <c r="V6" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E6,U6/100,ISERROR(F6))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W6" s="84"/>
       <c r="X6" s="281"/>
@@ -21536,10 +21536,10 @@
         <v>HKDAM1H6M=PREA</v>
       </c>
       <c r="M9" s="127">
-        <v>0.2</v>
+        <v>0.22</v>
       </c>
       <c r="N9" s="127">
-        <v>0.3</v>
+        <v>0.32</v>
       </c>
       <c r="O9" s="127">
         <v>0</v>
@@ -21549,19 +21549,19 @@
       </c>
       <c r="Q9" s="186">
         <f>_xll.qlMidSafe($M9,$N9)</f>
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="R9" s="88"/>
       <c r="S9" s="97">
-        <v>0.25</v>
+        <v>0.27</v>
       </c>
       <c r="T9" s="88"/>
       <c r="U9" s="156">
-        <v>0.25</v>
-      </c>
-      <c r="V9" s="94" t="e">
+        <v>0.27</v>
+      </c>
+      <c r="V9" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E9,U9/100,ISERROR(F9))</f>
-        <v>#N/A</v>
+        <v>2.0000000000000009E-4</v>
       </c>
       <c r="W9" s="84"/>
       <c r="X9" s="281"/>
@@ -21731,10 +21731,10 @@
         <v>HKDAM1H9M=PREA</v>
       </c>
       <c r="M12" s="127">
-        <v>0.24</v>
+        <v>0.27</v>
       </c>
       <c r="N12" s="127">
-        <v>0.34</v>
+        <v>0.37</v>
       </c>
       <c r="O12" s="127">
         <v>0</v>
@@ -21744,19 +21744,19 @@
       </c>
       <c r="Q12" s="186">
         <f>_xll.qlMidSafe($M12,$N12)</f>
-        <v>0.29000000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="R12" s="88"/>
       <c r="S12" s="97">
-        <v>0.29000000000000004</v>
+        <v>0.32</v>
       </c>
       <c r="T12" s="88"/>
       <c r="U12" s="156">
-        <v>0.29000000000000004</v>
-      </c>
-      <c r="V12" s="94" t="e">
+        <v>0.32</v>
+      </c>
+      <c r="V12" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E12,U12/100,ISERROR(F12))</f>
-        <v>#N/A</v>
+        <v>2.9999999999999992E-4</v>
       </c>
       <c r="W12" s="84"/>
       <c r="X12" s="281"/>
@@ -21926,10 +21926,10 @@
         <v>HKDAM1H1Y=PREA</v>
       </c>
       <c r="M15" s="133">
-        <v>0.28000000000000003</v>
+        <v>0.33</v>
       </c>
       <c r="N15" s="133">
-        <v>0.38</v>
+        <v>0.43</v>
       </c>
       <c r="O15" s="133">
         <v>0</v>
@@ -21939,19 +21939,19 @@
       </c>
       <c r="Q15" s="184">
         <f>_xll.qlMidSafe($M15,$N15)</f>
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="R15" s="88"/>
       <c r="S15" s="89">
-        <v>0.33</v>
+        <v>0.38</v>
       </c>
       <c r="T15" s="88"/>
       <c r="U15" s="149">
-        <v>0.33</v>
-      </c>
-      <c r="V15" s="85" t="e">
+        <v>0.38</v>
+      </c>
+      <c r="V15" s="85">
         <f>_xll.qlSimpleQuoteSetValue(E15,U15/100,ISERROR(F15))</f>
-        <v>#N/A</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="W15" s="84"/>
       <c r="X15" s="281"/>
@@ -22021,7 +22021,7 @@
   <sheetPr codeName="Sheet151"/>
   <dimension ref="A1:Z36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -22113,7 +22113,7 @@
       <c r="U3" s="146"/>
       <c r="V3" s="107">
         <f>_xll.ohTrigger(V5:V32)</f>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="W3" s="84"/>
       <c r="X3" s="116"/>
@@ -22146,7 +22146,7 @@
       <c r="K4" s="145"/>
       <c r="L4" s="106" t="str">
         <f>_xll.RData(L5:L35,M4:P4,,ReutersRtMode,,M5)</f>
-        <v>Paused at 11:12:44</v>
+        <v>Updated at 14:24:19</v>
       </c>
       <c r="M4" s="142" t="s">
         <v>157</v>
@@ -22213,10 +22213,10 @@
         <v>HKDQM3H6M=TRHK</v>
       </c>
       <c r="M5" s="127">
-        <v>0.35000000000000003</v>
+        <v>0.37</v>
       </c>
       <c r="N5" s="127">
-        <v>0.45</v>
+        <v>0.47000000000000003</v>
       </c>
       <c r="O5" s="127">
         <v>0</v>
@@ -22226,20 +22226,20 @@
       </c>
       <c r="Q5" s="90">
         <f>_xll.qlMidSafe($M5,$N5)</f>
-        <v>0.4</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="R5" s="88"/>
       <c r="S5" s="97">
-        <v>0.4</v>
+        <v>0.42000000000000004</v>
       </c>
       <c r="T5" s="88"/>
       <c r="U5" s="156">
         <f t="array" ref="U5:U35">QuoteLive</f>
-        <v>0.4</v>
-      </c>
-      <c r="V5" s="94" t="e">
+        <v>0.42000000000000004</v>
+      </c>
+      <c r="V5" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E5,U5/100,ISERROR(F5))</f>
-        <v>#N/A</v>
+        <v>2.0000000000000052E-4</v>
       </c>
       <c r="W5" s="84"/>
       <c r="X5" s="116"/>
@@ -22279,10 +22279,10 @@
         <v>HKDQM3H9M=TRHK</v>
       </c>
       <c r="M6" s="127">
-        <v>0.39</v>
+        <v>0.41000000000000003</v>
       </c>
       <c r="N6" s="127">
-        <v>0.49</v>
+        <v>0.51</v>
       </c>
       <c r="O6" s="127">
         <v>0</v>
@@ -22292,19 +22292,19 @@
       </c>
       <c r="Q6" s="90">
         <f>_xll.qlMidSafe($M6,$N6)</f>
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="R6" s="88"/>
       <c r="S6" s="97">
-        <v>0.44</v>
+        <v>0.46</v>
       </c>
       <c r="T6" s="88"/>
       <c r="U6" s="156">
-        <v>0.44</v>
-      </c>
-      <c r="V6" s="94" t="e">
+        <v>0.46</v>
+      </c>
+      <c r="V6" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E6,U6/100,ISERROR(F6))</f>
-        <v>#N/A</v>
+        <v>1.9999999999999966E-4</v>
       </c>
       <c r="W6" s="84"/>
       <c r="X6" s="116"/>
@@ -22344,10 +22344,10 @@
         <v>HKDQM3H1Y=TRHK</v>
       </c>
       <c r="M7" s="127">
-        <v>0.43</v>
+        <v>0.48</v>
       </c>
       <c r="N7" s="127">
-        <v>0.53</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="O7" s="127">
         <v>0</v>
@@ -22357,19 +22357,19 @@
       </c>
       <c r="Q7" s="90">
         <f>_xll.qlMidSafe($M7,$N7)</f>
-        <v>0.48</v>
+        <v>0.53</v>
       </c>
       <c r="R7" s="88"/>
       <c r="S7" s="97">
-        <v>0.48</v>
+        <v>0.53</v>
       </c>
       <c r="T7" s="88"/>
       <c r="U7" s="156">
-        <v>0.48</v>
-      </c>
-      <c r="V7" s="94" t="e">
+        <v>0.53</v>
+      </c>
+      <c r="V7" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E7,U7/100,ISERROR(F7))</f>
-        <v>#N/A</v>
+        <v>5.0000000000000044E-4</v>
       </c>
       <c r="W7" s="84"/>
       <c r="X7" s="116"/>
@@ -22474,10 +22474,10 @@
         <v>HKDQM3H18M=TRHK</v>
       </c>
       <c r="M9" s="127">
-        <v>0.6</v>
+        <v>0.62</v>
       </c>
       <c r="N9" s="127">
-        <v>0.70000000000000007</v>
+        <v>0.72</v>
       </c>
       <c r="O9" s="127">
         <v>0</v>
@@ -22487,19 +22487,19 @@
       </c>
       <c r="Q9" s="90">
         <f>_xll.qlMidSafe($M9,$N9)</f>
-        <v>0.65</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="R9" s="88"/>
       <c r="S9" s="97">
-        <v>0.65</v>
+        <v>0.66999999999999993</v>
       </c>
       <c r="T9" s="88"/>
       <c r="U9" s="156">
-        <v>0.65</v>
-      </c>
-      <c r="V9" s="94" t="e">
+        <v>0.66999999999999993</v>
+      </c>
+      <c r="V9" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E9,U9/100,ISERROR(F9))</f>
-        <v>#N/A</v>
+        <v>1.9999999999999879E-4</v>
       </c>
       <c r="W9" s="84"/>
       <c r="X9" s="116"/>
@@ -22627,9 +22627,9 @@
       <c r="U11" s="156">
         <v>0.83000000000000007</v>
       </c>
-      <c r="V11" s="94" t="e">
+      <c r="V11" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E11,U11/100,ISERROR(F11))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W11" s="84"/>
       <c r="X11" s="116"/>
@@ -22692,9 +22692,9 @@
       <c r="U12" s="156">
         <v>1.1400000000000001</v>
       </c>
-      <c r="V12" s="94" t="e">
+      <c r="V12" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E12,U12/100,ISERROR(F12))</f>
-        <v>#N/A</v>
+        <v>0</v>
       </c>
       <c r="W12" s="84"/>
       <c r="X12" s="116"/>
@@ -22734,10 +22734,10 @@
         <v>HKDQM3H4Y=TRHK</v>
       </c>
       <c r="M13" s="127">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
       <c r="N13" s="127">
-        <v>1.43</v>
+        <v>1.44</v>
       </c>
       <c r="O13" s="127">
         <v>0</v>
@@ -22747,19 +22747,19 @@
       </c>
       <c r="Q13" s="90">
         <f>_xll.qlMidSafe($M13,$N13)</f>
-        <v>1.38</v>
+        <v>1.3900000000000001</v>
       </c>
       <c r="R13" s="88"/>
       <c r="S13" s="97">
-        <v>1.38</v>
+        <v>1.3900000000000001</v>
       </c>
       <c r="T13" s="88"/>
       <c r="U13" s="156">
-        <v>1.38</v>
-      </c>
-      <c r="V13" s="94" t="e">
+        <v>1.3900000000000001</v>
+      </c>
+      <c r="V13" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E13,U13/100,ISERROR(F13))</f>
-        <v>#N/A</v>
+        <v>1.0000000000000113E-4</v>
       </c>
       <c r="W13" s="84"/>
       <c r="X13" s="116"/>
@@ -22799,10 +22799,10 @@
         <v>HKDQM3H5Y=TRHK</v>
       </c>
       <c r="M14" s="127">
-        <v>1.51</v>
+        <v>1.57</v>
       </c>
       <c r="N14" s="127">
-        <v>1.61</v>
+        <v>1.67</v>
       </c>
       <c r="O14" s="127">
         <v>0</v>
@@ -22812,19 +22812,19 @@
       </c>
       <c r="Q14" s="90">
         <f>_xll.qlMidSafe($M14,$N14)</f>
-        <v>1.56</v>
+        <v>1.62</v>
       </c>
       <c r="R14" s="88"/>
       <c r="S14" s="97">
-        <v>1.56</v>
+        <v>1.62</v>
       </c>
       <c r="T14" s="88"/>
       <c r="U14" s="156">
-        <v>1.56</v>
-      </c>
-      <c r="V14" s="94" t="e">
+        <v>1.62</v>
+      </c>
+      <c r="V14" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E14,U14/100,ISERROR(F14))</f>
-        <v>#N/A</v>
+        <v>6.0000000000000157E-4</v>
       </c>
       <c r="W14" s="84"/>
       <c r="X14" s="116"/>
@@ -22929,10 +22929,10 @@
         <v>HKDQM3H7Y=TRHK</v>
       </c>
       <c r="M16" s="127">
-        <v>1.77</v>
+        <v>1.8800000000000001</v>
       </c>
       <c r="N16" s="127">
-        <v>1.87</v>
+        <v>1.98</v>
       </c>
       <c r="O16" s="127">
         <v>0</v>
@@ -22942,19 +22942,19 @@
       </c>
       <c r="Q16" s="90">
         <f>_xll.qlMidSafe($M16,$N16)</f>
-        <v>1.82</v>
+        <v>1.9300000000000002</v>
       </c>
       <c r="R16" s="88"/>
       <c r="S16" s="97">
-        <v>1.82</v>
+        <v>1.9300000000000002</v>
       </c>
       <c r="T16" s="88"/>
       <c r="U16" s="156">
-        <v>1.82</v>
-      </c>
-      <c r="V16" s="94" t="e">
+        <v>1.9300000000000002</v>
+      </c>
+      <c r="V16" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E16,U16/100,ISERROR(F16))</f>
-        <v>#N/A</v>
+        <v>1.1000000000000003E-3</v>
       </c>
       <c r="W16" s="84"/>
       <c r="X16" s="116"/>
@@ -23124,10 +23124,10 @@
         <v>HKDQM3H10Y=TRHK</v>
       </c>
       <c r="M19" s="127">
-        <v>2.0100000000000002</v>
+        <v>2.16</v>
       </c>
       <c r="N19" s="127">
-        <v>2.11</v>
+        <v>2.2600000000000002</v>
       </c>
       <c r="O19" s="127">
         <v>0</v>
@@ -23137,19 +23137,19 @@
       </c>
       <c r="Q19" s="90">
         <f>_xll.qlMidSafe($M19,$N19)</f>
-        <v>2.06</v>
+        <v>2.21</v>
       </c>
       <c r="R19" s="88"/>
       <c r="S19" s="97">
-        <v>2.06</v>
+        <v>2.21</v>
       </c>
       <c r="T19" s="88"/>
       <c r="U19" s="156">
-        <v>2.06</v>
-      </c>
-      <c r="V19" s="94" t="e">
+        <v>2.21</v>
+      </c>
+      <c r="V19" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E19,U19/100,ISERROR(F19))</f>
-        <v>#N/A</v>
+        <v>1.4999999999999979E-3</v>
       </c>
       <c r="W19" s="84"/>
       <c r="X19" s="116"/>
@@ -23254,10 +23254,10 @@
         <v>HKDQM3H12Y=TRHK</v>
       </c>
       <c r="M21" s="127">
-        <v>2.09</v>
+        <v>2.2200000000000002</v>
       </c>
       <c r="N21" s="127">
-        <v>2.19</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="O21" s="127">
         <v>0</v>
@@ -23267,19 +23267,19 @@
       </c>
       <c r="Q21" s="90">
         <f>_xll.qlMidSafe($M21,$N21)</f>
-        <v>2.1399999999999997</v>
+        <v>2.27</v>
       </c>
       <c r="R21" s="88"/>
       <c r="S21" s="97">
-        <v>2.1399999999999997</v>
+        <v>2.27</v>
       </c>
       <c r="T21" s="88"/>
       <c r="U21" s="156">
-        <v>2.1399999999999997</v>
-      </c>
-      <c r="V21" s="94" t="e">
+        <v>2.27</v>
+      </c>
+      <c r="V21" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E21,U21/100,ISERROR(F21))</f>
-        <v>#N/A</v>
+        <v>1.300000000000006E-3</v>
       </c>
       <c r="W21" s="84"/>
       <c r="X21" s="116"/>
@@ -23449,10 +23449,10 @@
         <v>HKDQM3H15Y=TRHK</v>
       </c>
       <c r="M24" s="127">
-        <v>2.17</v>
+        <v>2.3199999999999998</v>
       </c>
       <c r="N24" s="127">
-        <v>2.27</v>
+        <v>2.42</v>
       </c>
       <c r="O24" s="127">
         <v>0</v>
@@ -23462,19 +23462,19 @@
       </c>
       <c r="Q24" s="90">
         <f>_xll.qlMidSafe($M24,$N24)</f>
-        <v>2.2199999999999998</v>
+        <v>2.37</v>
       </c>
       <c r="R24" s="88"/>
       <c r="S24" s="97">
-        <v>2.2199999999999998</v>
+        <v>2.37</v>
       </c>
       <c r="T24" s="88"/>
       <c r="U24" s="156">
-        <v>2.2199999999999998</v>
-      </c>
-      <c r="V24" s="94" t="e">
+        <v>2.37</v>
+      </c>
+      <c r="V24" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E24,U24/100,ISERROR(F24))</f>
-        <v>#N/A</v>
+        <v>1.5000000000000048E-3</v>
       </c>
       <c r="W24" s="84"/>
       <c r="X24" s="116"/>
@@ -23774,10 +23774,10 @@
         <v>HKDQM3H20Y=TRHK</v>
       </c>
       <c r="M29" s="127">
-        <v>2.25</v>
+        <v>2.4</v>
       </c>
       <c r="N29" s="127">
-        <v>2.4500000000000002</v>
+        <v>2.6</v>
       </c>
       <c r="O29" s="127">
         <v>0</v>
@@ -23787,19 +23787,19 @@
       </c>
       <c r="Q29" s="90">
         <f>_xll.qlMidSafe($M29,$N29)</f>
-        <v>2.35</v>
+        <v>2.5</v>
       </c>
       <c r="R29" s="88"/>
       <c r="S29" s="97">
-        <v>2.35</v>
+        <v>2.5</v>
       </c>
       <c r="T29" s="88"/>
       <c r="U29" s="156">
-        <v>2.35</v>
-      </c>
-      <c r="V29" s="94" t="e">
+        <v>2.5</v>
+      </c>
+      <c r="V29" s="94">
         <f>_xll.qlSimpleQuoteSetValue(E29,U29/100,ISERROR(F29))</f>
-        <v>#N/A</v>
+        <v>1.5000000000000013E-3</v>
       </c>
       <c r="W29" s="84"/>
       <c r="X29" s="116"/>

</xml_diff>